<commit_message>
added course descriptions in sucha way to have 3000 dim vectors
</commit_message>
<xml_diff>
--- a/AIacademia/data_files/countsentencespercoursename.xlsx
+++ b/AIacademia/data_files/countsentencespercoursename.xlsx
@@ -473,7 +473,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -499,7 +499,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -538,7 +538,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -564,7 +564,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -603,7 +603,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -629,7 +629,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -642,7 +642,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -655,7 +655,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -668,7 +668,7 @@
         <v>10</v>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -681,7 +681,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -707,7 +707,7 @@
         <v>11</v>
       </c>
       <c r="C21" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
@@ -720,7 +720,7 @@
         <v>10</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
@@ -733,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24">
@@ -785,7 +785,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28">
@@ -798,7 +798,7 @@
         <v>17</v>
       </c>
       <c r="C28" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
@@ -837,7 +837,7 @@
         <v>10</v>
       </c>
       <c r="C31" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
@@ -863,7 +863,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34">
@@ -954,7 +954,7 @@
         <v>10</v>
       </c>
       <c r="C40" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41">
@@ -1019,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="C45" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46">
@@ -1045,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48">
@@ -1071,7 +1071,7 @@
         <v>11</v>
       </c>
       <c r="C49" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50">
@@ -1097,7 +1097,7 @@
         <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52">
@@ -1110,7 +1110,7 @@
         <v>10</v>
       </c>
       <c r="C52" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53">
@@ -1123,7 +1123,7 @@
         <v>10</v>
       </c>
       <c r="C53" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54">
@@ -1149,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="C55" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56">
@@ -1162,7 +1162,7 @@
         <v>11</v>
       </c>
       <c r="C56" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57">
@@ -1201,7 +1201,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60">
@@ -1211,10 +1211,10 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C60" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61">
@@ -1227,7 +1227,7 @@
         <v>11</v>
       </c>
       <c r="C61" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62">
@@ -1266,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65">
@@ -1318,7 +1318,7 @@
         <v>10</v>
       </c>
       <c r="C68" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69">
@@ -1331,7 +1331,7 @@
         <v>12</v>
       </c>
       <c r="C69" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70">
@@ -1344,7 +1344,7 @@
         <v>10</v>
       </c>
       <c r="C70" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71">
@@ -1370,7 +1370,7 @@
         <v>13</v>
       </c>
       <c r="C72" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73">
@@ -1448,7 +1448,7 @@
         <v>13</v>
       </c>
       <c r="C78" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementing 4 similarity scores
</commit_message>
<xml_diff>
--- a/AIacademia/data_files/countsentencespercoursename.xlsx
+++ b/AIacademia/data_files/countsentencespercoursename.xlsx
@@ -456,11 +456,15 @@
           <t>Bachelor of Science (Agribusiness Management, With IT)</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C2" t="n">
-        <v>10</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -469,11 +473,15 @@
           <t>Bachelor of Science (Agricultural Economics, With IT)</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>20</v>
-      </c>
-      <c r="C3" t="n">
-        <v>10</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -482,11 +490,15 @@
           <t>Bachelor of Science (Agriculture Education and Extension, With IT)</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>11</v>
-      </c>
-      <c r="C4" t="n">
-        <v>15</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -495,11 +507,15 @@
           <t>Bachelor of Science (Agronomy, With IT)</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
-        <v>15</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -508,11 +524,15 @@
           <t>Bachelor of Science (Animal Science, With IT)</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>10</v>
-      </c>
-      <c r="C6" t="n">
-        <v>19</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -521,11 +541,15 @@
           <t>Bachelor of Science (Fisheries and Aquaculture, With IT)</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>10</v>
-      </c>
-      <c r="C7" t="n">
-        <v>12</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -534,11 +558,15 @@
           <t>Bachelor of Science (Horticulture, With IT)</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
-        <v>13</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -547,11 +575,15 @@
           <t>Bachelor of Science (Geography and Natural Resource Management, With IT)</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>14</v>
-      </c>
-      <c r="C9" t="n">
-        <v>18</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -560,11 +592,15 @@
           <t>Bachelor of Science (Climate Change and Development, With IT)</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" t="n">
-        <v>10</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -573,11 +609,15 @@
           <t>Bachelor of Arts (Communication &amp; Media Technology, With IT)</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="n">
-        <v>12</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -586,11 +626,15 @@
           <t>Bachelor of Arts (Criminology, With IT)</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>14</v>
-      </c>
-      <c r="C12" t="n">
-        <v>16</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -599,11 +643,15 @@
           <t>Bachelor of Arts (Drama and Theatre Studies, With IT)</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>13</v>
-      </c>
-      <c r="C13" t="n">
-        <v>13</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -612,11 +660,15 @@
           <t>Bachelor of Arts (Fine Art, With IT)</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>19</v>
-      </c>
-      <c r="C14" t="n">
-        <v>14</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -625,11 +677,15 @@
           <t>Bachelor of Arts (French, With IT)</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>10</v>
-      </c>
-      <c r="C15" t="n">
-        <v>12</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -638,11 +694,15 @@
           <t>Bachelor of Arts (History and Archaeology, With IT)</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>10</v>
-      </c>
-      <c r="C16" t="n">
-        <v>10</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -651,11 +711,15 @@
           <t>Bachelor of Arts (Interior Design, With IT)</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>15</v>
-      </c>
-      <c r="C17" t="n">
-        <v>13</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -664,11 +728,15 @@
           <t>Bachelor of Arts (Kiswahili, With IT)</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>10</v>
-      </c>
-      <c r="C18" t="n">
-        <v>12</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -677,11 +745,15 @@
           <t>Bachelor of Arts (Language and Communication, With IT)</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>10</v>
-      </c>
-      <c r="C19" t="n">
-        <v>10</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -690,11 +762,15 @@
           <t>Bachelor of Arts (Literature, With IT)</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>12</v>
-      </c>
-      <c r="C20" t="n">
-        <v>19</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -703,11 +779,15 @@
           <t>Bachelor of Arts (Music, With IT)</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>11</v>
-      </c>
-      <c r="C21" t="n">
-        <v>15</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -716,11 +796,15 @@
           <t>Bachelor of Arts (Philosophy, With IT)</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>10</v>
-      </c>
-      <c r="C22" t="n">
-        <v>10</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -729,11 +813,15 @@
           <t>Bachelor of Arts (Religion, With IT)</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>10</v>
-      </c>
-      <c r="C23" t="n">
-        <v>20</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -742,11 +830,15 @@
           <t>Bachelor of Arts (Sociology and Anthropology, With IT)</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>10</v>
-      </c>
-      <c r="C24" t="n">
-        <v>121</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -755,11 +847,15 @@
           <t>Bachelor of Arts (Textiles, Apparel Design and Fashion Merchandising, With IT)</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>16</v>
-      </c>
-      <c r="C25" t="n">
-        <v>17</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -768,11 +864,15 @@
           <t>Bachelor of Arts (Counseling Psychology, with IT)</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>10</v>
-      </c>
-      <c r="C26" t="n">
-        <v>10</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -781,11 +881,15 @@
           <t>Bachelor of Arts (With IT)</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>10</v>
-      </c>
-      <c r="C27" t="n">
-        <v>18</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -794,11 +898,15 @@
           <t>Bachelor of Arts (Business Studies, With IT)</t>
         </is>
       </c>
-      <c r="B28" t="n">
-        <v>17</v>
-      </c>
-      <c r="C28" t="n">
-        <v>15</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -807,11 +915,15 @@
           <t>Bachelor of Arts (Economics, With IT)</t>
         </is>
       </c>
-      <c r="B29" t="n">
-        <v>10</v>
-      </c>
-      <c r="C29" t="n">
-        <v>24</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -820,11 +932,15 @@
           <t>Bachelor of Business Administration (With IT)</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>15</v>
-      </c>
-      <c r="C30" t="n">
-        <v>48</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -833,11 +949,15 @@
           <t>Bachelor of Procurement and Supply Chain Management</t>
         </is>
       </c>
-      <c r="B31" t="n">
-        <v>10</v>
-      </c>
-      <c r="C31" t="n">
-        <v>10</v>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -846,11 +966,15 @@
           <t>Bachelor of Business Entrepreneurship, with IT</t>
         </is>
       </c>
-      <c r="B32" t="n">
-        <v>11</v>
-      </c>
-      <c r="C32" t="n">
-        <v>11</v>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -859,11 +983,15 @@
           <t>Bachelor of Science in Human Resource Management</t>
         </is>
       </c>
-      <c r="B33" t="n">
-        <v>11</v>
-      </c>
-      <c r="C33" t="n">
-        <v>16</v>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -872,11 +1000,15 @@
           <t>Bachelor of Science in Marketing, with IT</t>
         </is>
       </c>
-      <c r="B34" t="n">
-        <v>10</v>
-      </c>
-      <c r="C34" t="n">
-        <v>26</v>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -885,11 +1017,15 @@
           <t>Bachelor of Science in Accounting &amp; Finance, with IT</t>
         </is>
       </c>
-      <c r="B35" t="n">
-        <v>10</v>
-      </c>
-      <c r="C35" t="n">
-        <v>13</v>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -898,11 +1034,15 @@
           <t>Bachelor of Applied Economics with IT</t>
         </is>
       </c>
-      <c r="B36" t="n">
-        <v>15</v>
-      </c>
-      <c r="C36" t="n">
-        <v>13</v>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -911,11 +1051,15 @@
           <t>Bachelor of Economics &amp; Statistics, with IT</t>
         </is>
       </c>
-      <c r="B37" t="n">
-        <v>11</v>
-      </c>
-      <c r="C37" t="n">
-        <v>13</v>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -924,11 +1068,15 @@
           <t>Bachelor of Economics &amp; Finance with IT</t>
         </is>
       </c>
-      <c r="B38" t="n">
-        <v>10</v>
-      </c>
-      <c r="C38" t="n">
-        <v>12</v>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -937,11 +1085,15 @@
           <t>Bachelor of Science in Travel &amp; Tourism Management</t>
         </is>
       </c>
-      <c r="B39" t="n">
-        <v>10</v>
-      </c>
-      <c r="C39" t="n">
-        <v>16</v>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -950,11 +1102,15 @@
           <t>Bachelor of Science in Eco-tourism, Hotel and Institution Management</t>
         </is>
       </c>
-      <c r="B40" t="n">
-        <v>10</v>
-      </c>
-      <c r="C40" t="n">
-        <v>14</v>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -963,11 +1119,15 @@
           <t>Bachelor of Science (Information &amp; Communication Technology Management)</t>
         </is>
       </c>
-      <c r="B41" t="n">
-        <v>16</v>
-      </c>
-      <c r="C41" t="n">
-        <v>29</v>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -976,11 +1136,15 @@
           <t>Bachelor of Science (Information Technology)</t>
         </is>
       </c>
-      <c r="B42" t="n">
-        <v>15</v>
-      </c>
-      <c r="C42" t="n">
-        <v>14</v>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -989,11 +1153,15 @@
           <t>Bachelor of Science (Computer Science)</t>
         </is>
       </c>
-      <c r="B43" t="n">
-        <v>19</v>
-      </c>
-      <c r="C43" t="n">
-        <v>16</v>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1002,11 +1170,15 @@
           <t>Bachelor of Science (Computer Technology)</t>
         </is>
       </c>
-      <c r="B44" t="n">
-        <v>10</v>
-      </c>
-      <c r="C44" t="n">
-        <v>10</v>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -1015,11 +1187,15 @@
           <t>Bachelor of Science (Information Systems)</t>
         </is>
       </c>
-      <c r="B45" t="n">
-        <v>10</v>
-      </c>
-      <c r="C45" t="n">
-        <v>12</v>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1028,11 +1204,15 @@
           <t>Bachelor of Arts (International Relations and Diplomacy, With IT)</t>
         </is>
       </c>
-      <c r="B46" t="n">
-        <v>10</v>
-      </c>
-      <c r="C46" t="n">
-        <v>10</v>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1041,11 +1221,15 @@
           <t>Bachelor of Arts (Development Studies, With IT)</t>
         </is>
       </c>
-      <c r="B47" t="n">
-        <v>10</v>
-      </c>
-      <c r="C47" t="n">
-        <v>14</v>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -1054,11 +1238,15 @@
           <t>Bachelor of Arts (Political Science, With IT)</t>
         </is>
       </c>
-      <c r="B48" t="n">
-        <v>14</v>
-      </c>
-      <c r="C48" t="n">
-        <v>11</v>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -1067,11 +1255,15 @@
           <t>Bachelor of Education (Science, With IT)</t>
         </is>
       </c>
-      <c r="B49" t="n">
-        <v>11</v>
-      </c>
-      <c r="C49" t="n">
-        <v>15</v>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1080,11 +1272,15 @@
           <t>Bachelor of Education (Special Needs Education, With IT)</t>
         </is>
       </c>
-      <c r="B50" t="n">
-        <v>12</v>
-      </c>
-      <c r="C50" t="n">
-        <v>10</v>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -1093,11 +1289,15 @@
           <t>Bachelor of Education (Home Science, with IT)</t>
         </is>
       </c>
-      <c r="B51" t="n">
-        <v>10</v>
-      </c>
-      <c r="C51" t="n">
-        <v>16</v>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -1106,11 +1306,15 @@
           <t>Bachelor of Education (Early Childhood Education, With IT)</t>
         </is>
       </c>
-      <c r="B52" t="n">
-        <v>10</v>
-      </c>
-      <c r="C52" t="n">
-        <v>14</v>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -1119,11 +1323,15 @@
           <t>Bachelor of Education (French, With IT)</t>
         </is>
       </c>
-      <c r="B53" t="n">
-        <v>10</v>
-      </c>
-      <c r="C53" t="n">
-        <v>16</v>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -1132,11 +1340,15 @@
           <t>Bachelor of Education (Music, With IT)</t>
         </is>
       </c>
-      <c r="B54" t="n">
-        <v>10</v>
-      </c>
-      <c r="C54" t="n">
-        <v>15</v>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -1145,11 +1357,15 @@
           <t>Bachelor of Education (Arts, With IT)</t>
         </is>
       </c>
-      <c r="B55" t="n">
-        <v>11</v>
-      </c>
-      <c r="C55" t="n">
-        <v>30</v>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -1158,11 +1374,15 @@
           <t>Bachelor of Science (Actuarial Science, With IT)</t>
         </is>
       </c>
-      <c r="B56" t="n">
-        <v>11</v>
-      </c>
-      <c r="C56" t="n">
-        <v>16</v>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -1171,11 +1391,15 @@
           <t>Bachelor of Science (Applied Statistics, With IT)</t>
         </is>
       </c>
-      <c r="B57" t="n">
-        <v>10</v>
-      </c>
-      <c r="C57" t="n">
-        <v>11</v>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -1184,11 +1408,15 @@
           <t>Bachelor of Science (Mathematical Sciences, With IT)</t>
         </is>
       </c>
-      <c r="B58" t="n">
-        <v>10</v>
-      </c>
-      <c r="C58" t="n">
-        <v>16</v>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -1197,11 +1425,15 @@
           <t>Bachelor of Science (Mathematics &amp; Business Studies, With IT)</t>
         </is>
       </c>
-      <c r="B59" t="n">
-        <v>10</v>
-      </c>
-      <c r="C59" t="n">
-        <v>22</v>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -1210,11 +1442,15 @@
           <t>Bachelor of Science (Mathematics &amp; Computer Science)</t>
         </is>
       </c>
-      <c r="B60" t="n">
-        <v>20</v>
-      </c>
-      <c r="C60" t="n">
-        <v>23</v>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -1223,11 +1459,15 @@
           <t>Bachelor of Science (Mathematics &amp; Economics, With IT)</t>
         </is>
       </c>
-      <c r="B61" t="n">
-        <v>11</v>
-      </c>
-      <c r="C61" t="n">
-        <v>17</v>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -1236,11 +1476,15 @@
           <t>Bachelor of Medicine and Bachelor of Surgery (With IT)</t>
         </is>
       </c>
-      <c r="B62" t="n">
-        <v>27</v>
-      </c>
-      <c r="C62" t="n">
-        <v>11</v>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -1249,11 +1493,15 @@
           <t>Bachelor of Science (Biochemistry, With IT)</t>
         </is>
       </c>
-      <c r="B63" t="n">
-        <v>11</v>
-      </c>
-      <c r="C63" t="n">
-        <v>17</v>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -1262,11 +1510,15 @@
           <t>Bachelor of Science (Medical Laboratory Sciences, With IT)</t>
         </is>
       </c>
-      <c r="B64" t="n">
-        <v>10</v>
-      </c>
-      <c r="C64" t="n">
-        <v>15</v>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -1275,11 +1527,15 @@
           <t>Bachelor of Science (Nursing, With IT)</t>
         </is>
       </c>
-      <c r="B65" t="n">
-        <v>19</v>
-      </c>
-      <c r="C65" t="n">
-        <v>16</v>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -1288,11 +1544,15 @@
           <t>Bachelor of Pharmacy (With IT)</t>
         </is>
       </c>
-      <c r="B66" t="n">
-        <v>10</v>
-      </c>
-      <c r="C66" t="n">
-        <v>16</v>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -1301,11 +1561,15 @@
           <t>Bachelor of Science (Basic Science, With IT)</t>
         </is>
       </c>
-      <c r="B67" t="n">
-        <v>11</v>
-      </c>
-      <c r="C67" t="n">
-        <v>14</v>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -1314,11 +1578,15 @@
           <t>Bachelor of Science (Industrial Chemistry, With IT)</t>
         </is>
       </c>
-      <c r="B68" t="n">
-        <v>10</v>
-      </c>
-      <c r="C68" t="n">
-        <v>13</v>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -1327,11 +1595,15 @@
           <t>Bachelor of Science (Analytical Chemistry, with IT)</t>
         </is>
       </c>
-      <c r="B69" t="n">
-        <v>12</v>
-      </c>
-      <c r="C69" t="n">
-        <v>12</v>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -1340,11 +1612,15 @@
           <t>Bachelor of Science (Physics, with IT)</t>
         </is>
       </c>
-      <c r="B70" t="n">
-        <v>10</v>
-      </c>
-      <c r="C70" t="n">
-        <v>13</v>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -1353,11 +1629,15 @@
           <t>Bachelor of Science (Geospatial Information Science, With IT)</t>
         </is>
       </c>
-      <c r="B71" t="n">
-        <v>10</v>
-      </c>
-      <c r="C71" t="n">
-        <v>15</v>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -1366,11 +1646,15 @@
           <t>Bachelor of Arts (Urban and Regional Planning, With IT)</t>
         </is>
       </c>
-      <c r="B72" t="n">
-        <v>13</v>
-      </c>
-      <c r="C72" t="n">
-        <v>10</v>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -1379,11 +1663,15 @@
           <t>Bachelor of Arts (Disaster Management, With IT)</t>
         </is>
       </c>
-      <c r="B73" t="n">
-        <v>10</v>
-      </c>
-      <c r="C73" t="n">
-        <v>13</v>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -1392,11 +1680,15 @@
           <t>Bachelor of Science (Medical Biotechnology, With IT)</t>
         </is>
       </c>
-      <c r="B74" t="n">
-        <v>11</v>
-      </c>
-      <c r="C74" t="n">
-        <v>11</v>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -1405,11 +1697,15 @@
           <t>Bachelor of Science (Nutrition and Dietetics, With IT)</t>
         </is>
       </c>
-      <c r="B75" t="n">
-        <v>10</v>
-      </c>
-      <c r="C75" t="n">
-        <v>14</v>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -1418,11 +1714,15 @@
           <t>Bachelor of Science (Public Health, With IT)</t>
         </is>
       </c>
-      <c r="B76" t="n">
-        <v>10</v>
-      </c>
-      <c r="C76" t="n">
-        <v>26</v>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -1431,11 +1731,15 @@
           <t>Bachelor of Science (Health Records, with IT)</t>
         </is>
       </c>
-      <c r="B77" t="n">
-        <v>16</v>
-      </c>
-      <c r="C77" t="n">
-        <v>14</v>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
     <row r="78">
@@ -1444,11 +1748,15 @@
           <t>Bachelor of Laws (LLB)</t>
         </is>
       </c>
-      <c r="B78" t="n">
-        <v>13</v>
-      </c>
-      <c r="C78" t="n">
-        <v>14</v>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>['good']</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>